<commit_message>
Update examples. Set of small tweaks all intended to improve the examples
</commit_message>
<xml_diff>
--- a/Deliverables/IG/examples/Roche Phase 3 NCT04320615.xlsx
+++ b/Deliverables/IG/examples/Roche Phase 3 NCT04320615.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEAE84B-55E1-8B49-86EF-2768023BC062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C18EF95-2645-8145-A7FC-EF41709BAC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45060" yWindow="7800" windowWidth="56520" windowHeight="19480" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="37280" yWindow="4440" windowWidth="56520" windowHeight="19480" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
-    <sheet name="mainTimeline" sheetId="1" r:id="rId4"/>
-    <sheet name="studyDesignII" sheetId="6" r:id="rId5"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId6"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId7"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId8"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId9"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId10"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId11"/>
-    <sheet name="configuration" sheetId="10" r:id="rId12"/>
+    <sheet name="studyDesignArms" sheetId="15" r:id="rId4"/>
+    <sheet name="studyDesignEpochs" sheetId="14" r:id="rId5"/>
+    <sheet name="mainTimeline" sheetId="1" r:id="rId6"/>
+    <sheet name="studyDesignII" sheetId="6" r:id="rId7"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId8"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId9"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId10"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId11"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId12"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId13"/>
+    <sheet name="configuration" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="358">
   <si>
     <t>Epoch</t>
   </si>
@@ -1052,6 +1054,75 @@
   </si>
   <si>
     <t>Test Nine</t>
+  </si>
+  <si>
+    <t>FOLLOW-UP</t>
+  </si>
+  <si>
+    <t>Follow-up Epoch</t>
+  </si>
+  <si>
+    <t>TREATMENT</t>
+  </si>
+  <si>
+    <t>Treatment Epoch</t>
+  </si>
+  <si>
+    <t>BASELINE</t>
+  </si>
+  <si>
+    <t>Baseline Epoch</t>
+  </si>
+  <si>
+    <t>SCREENING</t>
+  </si>
+  <si>
+    <t>Screening Epoch</t>
+  </si>
+  <si>
+    <t>studyEpochType</t>
+  </si>
+  <si>
+    <t>studyEpochDescription</t>
+  </si>
+  <si>
+    <t>studyEpochName</t>
+  </si>
+  <si>
+    <t>studyArmName</t>
+  </si>
+  <si>
+    <t>studyArmDescription</t>
+  </si>
+  <si>
+    <t>studyArmType</t>
+  </si>
+  <si>
+    <t>studyArmDataOriginDescription</t>
+  </si>
+  <si>
+    <t>studyArmDataOriginType</t>
+  </si>
+  <si>
+    <t>Active Comparator Arm</t>
+  </si>
+  <si>
+    <t>Data collected from subjects</t>
+  </si>
+  <si>
+    <t>Data Generated Within Study</t>
+  </si>
+  <si>
+    <t>Placebo Comparator Arm</t>
+  </si>
+  <si>
+    <t>Tocilizumab with Standard of Care</t>
+  </si>
+  <si>
+    <t>Placebo with Standard of Care</t>
+  </si>
+  <si>
+    <t>Completion Epoch</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1230,6 +1301,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1548,7 +1622,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1716,6 +1790,172 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="61.83203125" customWidth="1"/>
+    <col min="7" max="8" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24" style="29" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4E9D5-B601-284A-9651-0AA604C2B9D1}">
   <dimension ref="A1:AF36"/>
   <sheetViews>
@@ -2502,7 +2742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FA5DC6-70BE-E845-A085-20526138A835}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2625,7 +2865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2759,8 +2999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F3"/>
+    <sheetView topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2967,6 +3207,173 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A249A8FC-0BFB-B542-9B53-D076A9E0F532}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D777F3-5BEA-F342-A5A3-C0203B86F3C9}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:AO36"/>
   <sheetViews>
@@ -6932,7 +7339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FA45D-9570-C643-AC7B-6310BD62121C}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -7022,7 +7429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -7078,7 +7485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -7593,170 +8000,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
-    <col min="7" max="8" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24" style="29" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>329</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>330</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B3" t="s">
-        <v>333</v>
-      </c>
-      <c r="C3" t="s">
-        <v>334</v>
-      </c>
-      <c r="D3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="G3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D5" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>